<commit_message>
Update artefato 17 e 19
</commit_message>
<xml_diff>
--- a/artefatos/17. Análise dos Eventos para cada Cenário.xlsx
+++ b/artefatos/17. Análise dos Eventos para cada Cenário.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e90e968d6f8cb6a5/Documentos/^N Faculdade/OPE/smart-owl/Artefatos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Faculdade\Engenharia\hairtech\artefatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1BE8D25B-225C-4F68-A6BA-8A26254D18C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
     <sheet name="Plan2" sheetId="2" r:id="rId2"/>
     <sheet name="Plan3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -128,9 +127,6 @@
     <t>x (8)</t>
   </si>
   <si>
-    <t>Realizar finalização solicitada pelo cliente</t>
-  </si>
-  <si>
     <t>x (9)</t>
   </si>
   <si>
@@ -150,13 +146,16 @@
   </si>
   <si>
     <t>x (12)</t>
+  </si>
+  <si>
+    <t>Realizar finalização do serviço</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -414,9 +413,6 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -436,6 +432,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -472,9 +471,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -512,7 +511,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -547,23 +546,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -599,26 +581,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -791,14 +756,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.42578125" customWidth="1"/>
     <col min="2" max="2" width="5.140625" customWidth="1"/>
@@ -812,7 +777,7 @@
     <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="3" customFormat="1" ht="51" customHeight="1">
+    <row r="1" spans="1:10" s="3" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E1" s="28" t="s">
         <v>0</v>
       </c>
@@ -824,7 +789,7 @@
       <c r="I1" s="28"/>
       <c r="J1" s="2"/>
     </row>
-    <row r="2" spans="1:10" s="3" customFormat="1" ht="46.5" customHeight="1">
+    <row r="2" spans="1:10" s="3" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
         <v>2</v>
       </c>
@@ -854,7 +819,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="45.75" customHeight="1">
+    <row r="3" spans="1:10" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>11</v>
       </c>
@@ -876,7 +841,7 @@
       <c r="I3" s="9"/>
       <c r="J3" s="10"/>
     </row>
-    <row r="4" spans="1:10" ht="44.25" customHeight="1">
+    <row r="4" spans="1:10" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>15</v>
       </c>
@@ -898,11 +863,11 @@
       <c r="I4" s="5"/>
       <c r="J4" s="6"/>
     </row>
-    <row r="5" spans="1:10" ht="17.25" customHeight="1">
+    <row r="5" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="27" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="12">
@@ -920,9 +885,9 @@
       <c r="I5" s="5"/>
       <c r="J5" s="6"/>
     </row>
-    <row r="6" spans="1:10" ht="16.5" customHeight="1">
+    <row r="6" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="30"/>
-      <c r="B6" s="20"/>
+      <c r="B6" s="27"/>
       <c r="C6" s="12">
         <v>4</v>
       </c>
@@ -938,9 +903,9 @@
       <c r="I6" s="5"/>
       <c r="J6" s="6"/>
     </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1">
+    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="30"/>
-      <c r="B7" s="20"/>
+      <c r="B7" s="27"/>
       <c r="C7" s="12">
         <v>5</v>
       </c>
@@ -956,9 +921,9 @@
       <c r="I7" s="5"/>
       <c r="J7" s="6"/>
     </row>
-    <row r="8" spans="1:10" ht="15.75" customHeight="1">
+    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="30"/>
-      <c r="B8" s="20"/>
+      <c r="B8" s="27"/>
       <c r="C8" s="12">
         <v>6</v>
       </c>
@@ -974,11 +939,11 @@
       <c r="I8" s="5"/>
       <c r="J8" s="6"/>
     </row>
-    <row r="9" spans="1:10" ht="15" customHeight="1">
-      <c r="A9" s="21" t="s">
+    <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="23" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="12">
@@ -996,9 +961,9 @@
       <c r="I9" s="5"/>
       <c r="J9" s="6"/>
     </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="22"/>
-      <c r="B10" s="25"/>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="21"/>
+      <c r="B10" s="24"/>
       <c r="C10" s="12">
         <v>8</v>
       </c>
@@ -1014,9 +979,9 @@
       <c r="I10" s="5"/>
       <c r="J10" s="6"/>
     </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="22"/>
-      <c r="B11" s="25"/>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="21"/>
+      <c r="B11" s="24"/>
       <c r="C11" s="12">
         <v>9</v>
       </c>
@@ -1032,17 +997,17 @@
       <c r="I11" s="5"/>
       <c r="J11" s="6"/>
     </row>
-    <row r="12" spans="1:10">
-      <c r="A12" s="23"/>
-      <c r="B12" s="26"/>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="22"/>
+      <c r="B12" s="25"/>
       <c r="C12" s="12">
         <v>10</v>
       </c>
       <c r="D12" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="14" t="s">
         <v>31</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>32</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="5"/>
@@ -1050,9 +1015,9 @@
       <c r="I12" s="5"/>
       <c r="J12" s="6"/>
     </row>
-    <row r="13" spans="1:10" ht="15" customHeight="1">
+    <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B13" s="12" t="s">
         <v>12</v>
@@ -1061,7 +1026,7 @@
         <v>11</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E13" s="14"/>
       <c r="F13" s="4"/>
@@ -1072,18 +1037,18 @@
       <c r="I13" s="5"/>
       <c r="J13" s="6"/>
     </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="20" t="s">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="27" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="12">
         <v>12</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="4" t="s">
@@ -1094,17 +1059,17 @@
       <c r="I14" s="5"/>
       <c r="J14" s="6"/>
     </row>
-    <row r="15" spans="1:10">
-      <c r="A15" s="27"/>
-      <c r="B15" s="20"/>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="26"/>
+      <c r="B15" s="27"/>
       <c r="C15" s="12">
         <v>13</v>
       </c>
       <c r="D15" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" s="14" t="s">
         <v>37</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>38</v>
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="5"/>
@@ -1112,50 +1077,49 @@
       <c r="I15" s="5"/>
       <c r="J15" s="6"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D16" s="11"/>
     </row>
-    <row r="19" spans="2:7">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G19"/>
     </row>
-    <row r="20" spans="2:7">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G20"/>
     </row>
-    <row r="21" spans="2:7">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="7"/>
       <c r="C21" s="3"/>
       <c r="G21"/>
     </row>
-    <row r="22" spans="2:7">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="7"/>
       <c r="C22" s="3"/>
       <c r="G22"/>
     </row>
-    <row r="23" spans="2:7">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="7"/>
       <c r="C23" s="3"/>
       <c r="G23"/>
     </row>
-    <row r="24" spans="2:7">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="7"/>
       <c r="C24" s="3"/>
       <c r="G24"/>
     </row>
-    <row r="25" spans="2:7">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="7"/>
       <c r="C25" s="3"/>
       <c r="G25"/>
     </row>
-    <row r="26" spans="2:7">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="G26"/>
     </row>
-    <row r="27" spans="2:7">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G27"/>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A5:A8"/>
@@ -1164,6 +1128,7 @@
     <mergeCell ref="B9:B12"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="B14:B15"/>
+    <mergeCell ref="E1:F1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1171,24 +1136,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>